<commit_message>
Scripting SCD0296 and SCD0297
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0296 - Penyelia, CRO CRM, SRM, Admin SLN, dan Admin WEM melakukan edit data Non Sales yang telah diajukan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0296 - Penyelia, CRO CRM, SRM, Admin SLN, dan Admin WEM melakukan edit data Non Sales yang telah diajukan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BD8B54-0C6A-4255-855D-5B5BC7E833C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21254F8-1142-4A50-AD32-5C306C7BE35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>RUN</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Admin WEM</t>
-  </si>
-  <si>
-    <t>Cuti Melahirkan</t>
   </si>
   <si>
     <t>DGS-311</t>
@@ -148,7 +145,7 @@
  -Klik save</t>
   </si>
   <si>
-    <t>TEXT7</t>
+    <t>Cuti Sakit,Cuti Melahirkan</t>
   </si>
 </sst>
 </file>
@@ -202,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -224,9 +221,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -543,7 +537,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,25 +615,22 @@
       <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="2" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F2" s="3">
         <v>32362</v>
@@ -648,24 +639,29 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="6"/>
+      <c r="L2" s="7">
+        <v>55210</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f ca="1">TEXT(TODAY(),"yyyy-mm-dd")</f>
+        <v>2022-09-07</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f ca="1">TEXT(TODAY()+2,"yyyy-mm-dd")</f>
+        <v>2022-09-09</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="7">
-        <v>369</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="R2" s="7"/>
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
@@ -673,16 +669,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3">
         <v>29349</v>
@@ -691,38 +687,44 @@
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="L3" s="8">
+        <v>29349</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M6" ca="1" si="0">TEXT(TODAY(),"yyyy-mm-dd")</f>
+        <v>2022-09-07</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" ref="N3:N6" ca="1" si="1">TEXT(TODAY()+2,"yyyy-mm-dd")</f>
+        <v>2022-09-09</v>
+      </c>
       <c r="O3" s="6"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="7">
-        <v>370</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
         <v>32587</v>
@@ -731,38 +733,44 @@
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="L4" s="8">
+        <v>32587</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2022-09-07</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2022-09-09</v>
+      </c>
       <c r="O4" s="6"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R4" s="7">
-        <v>407</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
         <v>37679</v>
@@ -776,33 +784,39 @@
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="L5" s="8">
+        <v>29029</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2022-09-07</v>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2022-09-09</v>
+      </c>
       <c r="O5" s="6"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" s="7">
-        <v>418</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3">
         <v>52326</v>
@@ -816,17 +830,23 @@
       <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="L6" s="9">
+        <v>55454</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2022-09-07</v>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2022-09-09</v>
+      </c>
       <c r="O6" s="6"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R6" s="7">
-        <v>417</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="R6" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>